<commit_message>
including the summary table
</commit_message>
<xml_diff>
--- a/Results/model_comparison_v2.xlsx
+++ b/Results/model_comparison_v2.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethbrasseale/Projects/eDNA/code/R/nimble/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36BA778-7DAD-0C4B-A8EB-60BA0960973B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4B3B6C-6D84-3F4E-AD39-C08066F9ADB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1560" windowWidth="28040" windowHeight="15560" xr2:uid="{BC6E49AD-47D7-F249-BF80-8BE9CE838060}"/>
+    <workbookView xWindow="4300" yWindow="2360" windowWidth="28040" windowHeight="15560" xr2:uid="{BC6E49AD-47D7-F249-BF80-8BE9CE838060}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nimble summary (m2x models)" sheetId="4" r:id="rId1"/>
-    <sheet name="Nimble priors (m2x models)" sheetId="6" r:id="rId2"/>
-    <sheet name="Nimble priors" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="Stan summary (w proc var)" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="Stan summary (no proc var)" sheetId="1" state="hidden" r:id="rId5"/>
-    <sheet name="Old priors" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Nimble summary (unit convert)" sheetId="10" r:id="rId1"/>
+    <sheet name="Nimble summary (m3x models)" sheetId="9" r:id="rId2"/>
+    <sheet name="Nimble priors (m3x models)" sheetId="8" r:id="rId3"/>
+    <sheet name="Nimble summary (m2x models)" sheetId="4" r:id="rId4"/>
+    <sheet name="Nimble priors (m2x models)" sheetId="6" r:id="rId5"/>
+    <sheet name="Nimble priors" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="Stan summary (w proc var)" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Stan summary (no proc var)" sheetId="1" state="hidden" r:id="rId8"/>
+    <sheet name="Old priors" sheetId="2" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="76">
   <si>
     <t>model name</t>
   </si>
@@ -236,13 +239,46 @@
   </si>
   <si>
     <t>(μ[t-1]+β)*⍺[t]</t>
+  </si>
+  <si>
+    <t>unif(1,10000)</t>
+  </si>
+  <si>
+    <t>xinit</t>
+  </si>
+  <si>
+    <t>unif(10,10000)</t>
+  </si>
+  <si>
+    <t>unif(0.01,10)</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>95%CI_low</t>
+  </si>
+  <si>
+    <t>95%CI_upp</t>
+  </si>
+  <si>
+    <t>68,45</t>
+  </si>
+  <si>
+    <t>0.29-0.73</t>
+  </si>
+  <si>
+    <t>0.01-0.26</t>
+  </si>
+  <si>
+    <t>0.91–0.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,16 +286,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -267,16 +316,178 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +801,1512 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CDEE08-6195-9E46-9B20-675E9C89CB78}">
+  <dimension ref="A1:AB8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AB2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="22"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="22"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="18"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="6">
+        <v>203</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1529</v>
+      </c>
+      <c r="G3" s="6">
+        <v>6.46</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3.33</v>
+      </c>
+      <c r="I3" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="J3" s="6">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K3" s="8">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1875</v>
+      </c>
+      <c r="N3" s="7">
+        <v>10.35</v>
+      </c>
+      <c r="O3" s="4">
+        <v>8847</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>358.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="6">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>181</v>
+      </c>
+      <c r="G4" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.185</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.87</v>
+      </c>
+      <c r="M4" s="6">
+        <v>14.56</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="4">
+        <v>56.7</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>355.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="6">
+        <v>181</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1399.7</v>
+      </c>
+      <c r="G5" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3.34</v>
+      </c>
+      <c r="I5" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="J5" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1723</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3.09</v>
+      </c>
+      <c r="O5" s="4">
+        <v>8795</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>358.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="6">
+        <v>13.2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.85</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.15</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="M6" s="6">
+        <v>4.59</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>16</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="6">
+        <v>185.5</v>
+      </c>
+      <c r="T6" s="7">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="U6" s="4">
+        <v>404.8</v>
+      </c>
+      <c r="V6" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W6" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="X6" s="4">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>321.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="6">
+        <v>139</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="F7" s="4">
+        <v>974</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3.29</v>
+      </c>
+      <c r="I7" s="4">
+        <v>9.74</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M7" s="6">
+        <v>485</v>
+      </c>
+      <c r="N7" s="7">
+        <v>7.09</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3484</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>-0.47</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>357.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>35</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="11">
+        <v>43</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1.41</v>
+      </c>
+      <c r="F8" s="9">
+        <v>256.89999999999998</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5.23</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9.4</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="11">
+        <v>14.7</v>
+      </c>
+      <c r="N8" s="12">
+        <v>6.6</v>
+      </c>
+      <c r="O8" s="9">
+        <v>28.2</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB8" s="10">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6F294D-6304-DD48-A7E4-EA8EF4A94450}">
+  <dimension ref="A1:AB8"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AF1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.33203125" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3">
+        <v>203</v>
+      </c>
+      <c r="E3">
+        <v>1.77</v>
+      </c>
+      <c r="F3">
+        <v>1529</v>
+      </c>
+      <c r="G3">
+        <v>6.46</v>
+      </c>
+      <c r="H3">
+        <v>3.33</v>
+      </c>
+      <c r="I3">
+        <v>9.75</v>
+      </c>
+      <c r="J3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="L3">
+        <v>0.48</v>
+      </c>
+      <c r="M3">
+        <v>1875</v>
+      </c>
+      <c r="N3">
+        <v>10.35</v>
+      </c>
+      <c r="O3">
+        <v>8847</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3">
+        <v>358.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>1.3</v>
+      </c>
+      <c r="F4">
+        <v>181</v>
+      </c>
+      <c r="G4">
+        <v>6.4</v>
+      </c>
+      <c r="H4">
+        <v>3.2</v>
+      </c>
+      <c r="I4">
+        <v>9.75</v>
+      </c>
+      <c r="J4">
+        <v>0.51</v>
+      </c>
+      <c r="K4">
+        <v>0.185</v>
+      </c>
+      <c r="L4">
+        <v>0.87</v>
+      </c>
+      <c r="M4">
+        <v>14.56</v>
+      </c>
+      <c r="N4">
+        <v>1.5</v>
+      </c>
+      <c r="O4">
+        <v>56.7</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4">
+        <v>355.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>181</v>
+      </c>
+      <c r="E5">
+        <v>1.7</v>
+      </c>
+      <c r="F5">
+        <v>1399.7</v>
+      </c>
+      <c r="G5">
+        <v>6.5</v>
+      </c>
+      <c r="H5">
+        <v>3.34</v>
+      </c>
+      <c r="I5">
+        <v>9.75</v>
+      </c>
+      <c r="J5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L5">
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <v>1723</v>
+      </c>
+      <c r="N5">
+        <v>3.09</v>
+      </c>
+      <c r="O5">
+        <v>8795</v>
+      </c>
+      <c r="P5">
+        <v>0.53</v>
+      </c>
+      <c r="Q5">
+        <v>0.22</v>
+      </c>
+      <c r="R5">
+        <v>1.43</v>
+      </c>
+      <c r="S5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5">
+        <v>358.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6">
+        <v>13.2</v>
+      </c>
+      <c r="E6">
+        <v>1.21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6">
+        <v>1.85</v>
+      </c>
+      <c r="H6">
+        <v>1.01</v>
+      </c>
+      <c r="I6">
+        <v>5.15</v>
+      </c>
+      <c r="J6">
+        <v>0.36</v>
+      </c>
+      <c r="K6">
+        <v>0.19</v>
+      </c>
+      <c r="L6">
+        <v>0.51</v>
+      </c>
+      <c r="M6">
+        <v>4.59</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>16</v>
+      </c>
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6">
+        <v>185.5</v>
+      </c>
+      <c r="T6">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="U6">
+        <v>404.8</v>
+      </c>
+      <c r="V6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W6">
+        <v>0.04</v>
+      </c>
+      <c r="X6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6">
+        <v>321.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>139</v>
+      </c>
+      <c r="E7">
+        <v>1.7</v>
+      </c>
+      <c r="F7">
+        <v>974</v>
+      </c>
+      <c r="G7">
+        <v>6.4</v>
+      </c>
+      <c r="H7">
+        <v>3.29</v>
+      </c>
+      <c r="I7">
+        <v>9.74</v>
+      </c>
+      <c r="J7">
+        <v>0.11</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M7">
+        <v>485</v>
+      </c>
+      <c r="N7">
+        <v>7.09</v>
+      </c>
+      <c r="O7">
+        <v>3484</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z7">
+        <v>-0.47</v>
+      </c>
+      <c r="AA7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AB7">
+        <v>357.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>43</v>
+      </c>
+      <c r="E8">
+        <v>1.41</v>
+      </c>
+      <c r="F8">
+        <v>256.89999999999998</v>
+      </c>
+      <c r="G8">
+        <v>5.23</v>
+      </c>
+      <c r="H8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I8">
+        <v>9.4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8">
+        <v>14.7</v>
+      </c>
+      <c r="N8">
+        <v>6.6</v>
+      </c>
+      <c r="O8">
+        <v>28.2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB8">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5B78AF-E3B5-994E-A98B-D4EADF85431F}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F70FFAA-C73E-A449-ABA6-38905378C8B2}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -898,7 +2611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF0ECC-E744-1F40-801E-866D196830AC}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -992,7 +2705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196D9CF8-DB76-864C-86D4-6F5210928883}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1072,7 +2785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64644ADB-F159-824E-8CB1-3FC7B4EDF34F}">
   <dimension ref="A1:P8"/>
   <sheetViews>
@@ -1445,7 +3158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A10F6E-60C2-D34D-AEF9-61F026003DBC}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -1828,7 +3541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690ECE77-C7E0-364C-A099-061D4F4F36C2}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>